<commit_message>
combined six new test items from David Lopez of AIR modified imsmanifest.xml accordingly
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/PT10thGradeMathItemsWithStudentResponses_1_13_15.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/PT10thGradeMathItemsWithStudentResponses_1_13_15.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="29025" windowHeight="27045" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13305" windowHeight="18495" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1163,7 +1164,7 @@
   <dimension ref="A1:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>